<commit_message>
csv copy to excel
</commit_message>
<xml_diff>
--- a/docs/modules/excel_utilities/another_folder/target.xlsx
+++ b/docs/modules/excel_utilities/another_folder/target.xlsx
@@ -1,27 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ACMA-ANSYS04\Data\github\assetutilities\docs\modules\documentation\excel_utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ACMA-ANSYS04\Data\github\assetutilities\docs\modules\excel_utilities\another_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555D09CF-6183-4327-AAF1-7E9F8F316704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3ECF86-F551-4B67-A604-86564FC840CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3375" windowWidth="19200" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transform" sheetId="1" r:id="rId1"/>
-    <sheet name="inputs" sheetId="3" r:id="rId2"/>
-    <sheet name="results" sheetId="2" r:id="rId3"/>
+    <sheet name="inputs" sheetId="2" r:id="rId2"/>
+    <sheet name="results" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -40,6 +37,93 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="133">
   <si>
+    <t>Revision</t>
+  </si>
+  <si>
+    <t>FST1</t>
+  </si>
+  <si>
+    <t>FST2</t>
+  </si>
+  <si>
+    <t>Tide</t>
+  </si>
+  <si>
+    <t>Loading Direction</t>
+  </si>
+  <si>
+    <t>Wind heading</t>
+  </si>
+  <si>
+    <t>Wind speed</t>
+  </si>
+  <si>
+    <t>Wave heading</t>
+  </si>
+  <si>
+    <t>Hs</t>
+  </si>
+  <si>
+    <t>Tz</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>Current speed</t>
+  </si>
+  <si>
+    <t>Current heading</t>
+  </si>
+  <si>
+    <t>FST2 - Strut Loads (kN)</t>
+  </si>
+  <si>
+    <t>FST1 - Strut Loads (kN)</t>
+  </si>
+  <si>
+    <t>%load</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Strut1</t>
+  </si>
+  <si>
+    <t>Strut2</t>
+  </si>
+  <si>
+    <t>Strut3</t>
+  </si>
+  <si>
+    <t>Strut4</t>
+  </si>
+  <si>
+    <t>Strut5</t>
+  </si>
+  <si>
+    <t>Strut6</t>
+  </si>
+  <si>
+    <t>Strut7</t>
+  </si>
+  <si>
+    <t>Strut8</t>
+  </si>
+  <si>
     <t>fe_filename</t>
   </si>
   <si>
@@ -52,6 +136,228 @@
     <t>statistic</t>
   </si>
   <si>
+    <t>FST1_Heading</t>
+  </si>
+  <si>
+    <t>FST2_Heading</t>
+  </si>
+  <si>
+    <t>WindDirection</t>
+  </si>
+  <si>
+    <t>WindSpeed</t>
+  </si>
+  <si>
+    <t>WaveDirection</t>
+  </si>
+  <si>
+    <t>WaveTz</t>
+  </si>
+  <si>
+    <t>WaveGamma</t>
+  </si>
+  <si>
+    <t>RefCurrentSpeed</t>
+  </si>
+  <si>
+    <t>RefCurrentDirection</t>
+  </si>
+  <si>
+    <t>CurrentFactor[0]</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_000deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_015deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_030deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_045deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_060deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_075deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_090deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_105deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_120deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_135deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_150deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_165deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_180deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_195deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_210deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_225deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_240deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_255deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_270deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_285deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_300deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_315deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_330deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_345deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_cl_015deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_cl_030deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_cl_045deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_cl_090deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_cl_180deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_000deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_015deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_030deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_045deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_060deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_075deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_090deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_105deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_120deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_135deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_150deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_165deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_180deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_195deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_210deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_225deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_240deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_255deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_270deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_285deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_300deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_315deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_330deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_345deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_cl_015deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_cl_030deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_cl_045deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_cl_090deg.sim</t>
+  </si>
+  <si>
+    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_cl_180deg.sim</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>stdev</t>
+  </si>
+  <si>
     <t>Strut1_Body_eff_tension_min</t>
   </si>
   <si>
@@ -128,322 +434,13 @@
   </si>
   <si>
     <t>K:/1522/ctr7/orcaflex/anl/fsts/5_seeds/FST2F_FST1F_LWL_300deg_S5.sim</t>
-  </si>
-  <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>stdev</t>
-  </si>
-  <si>
-    <t>FST1_Heading</t>
-  </si>
-  <si>
-    <t>FST2_Heading</t>
-  </si>
-  <si>
-    <t>WindDirection</t>
-  </si>
-  <si>
-    <t>WindSpeed</t>
-  </si>
-  <si>
-    <t>WaveDirection</t>
-  </si>
-  <si>
-    <t>Hs</t>
-  </si>
-  <si>
-    <t>WaveTz</t>
-  </si>
-  <si>
-    <t>WaveGamma</t>
-  </si>
-  <si>
-    <t>RefCurrentSpeed</t>
-  </si>
-  <si>
-    <t>RefCurrentDirection</t>
-  </si>
-  <si>
-    <t>CurrentFactor[0]</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_000deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_015deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_030deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_045deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_060deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_075deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_090deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_105deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_120deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_135deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_150deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_165deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_180deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_195deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_210deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_225deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_240deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_255deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_270deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_285deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_300deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_315deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_330deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_345deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_cl_015deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_cl_030deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_cl_045deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_cl_090deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2F_FST1F_LWL_cl_180deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_000deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_015deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_030deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_045deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_060deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_075deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_090deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_105deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_120deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_135deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_150deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_165deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_180deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_195deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_210deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_225deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_240deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_255deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_270deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_285deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_300deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_315deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_330deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_345deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_cl_015deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_cl_030deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_cl_045deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_cl_090deg.sim</t>
-  </si>
-  <si>
-    <t>K:/1522/ctr7/orcaflex/anl/fsts/FST2L_FST1L_HWL_cl_180deg.sim</t>
-  </si>
-  <si>
-    <t>Revision</t>
-  </si>
-  <si>
-    <t>FST1</t>
-  </si>
-  <si>
-    <t>FST2</t>
-  </si>
-  <si>
-    <t>Tide</t>
-  </si>
-  <si>
-    <t>Loading Direction</t>
-  </si>
-  <si>
-    <t>Wind heading</t>
-  </si>
-  <si>
-    <t>Wind speed</t>
-  </si>
-  <si>
-    <t>Wave heading</t>
-  </si>
-  <si>
-    <t>Tz</t>
-  </si>
-  <si>
-    <t>Gamma</t>
-  </si>
-  <si>
-    <t>Current speed</t>
-  </si>
-  <si>
-    <t>Current heading</t>
-  </si>
-  <si>
-    <t>FST2 - Strut Loads (kN)</t>
-  </si>
-  <si>
-    <t>FST1 - Strut Loads (kN)</t>
-  </si>
-  <si>
-    <t>%load</t>
-  </si>
-  <si>
-    <t>deg</t>
-  </si>
-  <si>
-    <t>m/s</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>Strut1</t>
-  </si>
-  <si>
-    <t>Strut2</t>
-  </si>
-  <si>
-    <t>Strut3</t>
-  </si>
-  <si>
-    <t>Strut4</t>
-  </si>
-  <si>
-    <t>Strut5</t>
-  </si>
-  <si>
-    <t>Strut6</t>
-  </si>
-  <si>
-    <t>Strut7</t>
-  </si>
-  <si>
-    <t>Strut8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,6 +474,11 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -498,7 +500,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -527,19 +529,6 @@
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -664,11 +653,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -676,26 +708,26 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -704,30 +736,30 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,7 +768,6 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
         <strike val="0"/>
         <color rgb="FFC00000"/>
       </font>
@@ -744,14 +775,12 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
         <color theme="7" tint="-0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
         <strike val="0"/>
         <color rgb="FFC00000"/>
       </font>
@@ -759,14 +788,12 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
         <color theme="7" tint="-0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
         <strike val="0"/>
         <color rgb="FFC00000"/>
       </font>
@@ -774,14 +801,12 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
         <color theme="7" tint="-0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
         <strike val="0"/>
         <color rgb="FFC00000"/>
       </font>
@@ -789,14 +814,12 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
         <color theme="7" tint="-0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
         <strike val="0"/>
         <color rgb="FFC00000"/>
       </font>
@@ -804,14 +827,12 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
         <color theme="7" tint="-0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
         <strike val="0"/>
         <color rgb="FFC00000"/>
       </font>
@@ -819,14 +840,12 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
         <color theme="7" tint="-0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
         <strike val="0"/>
         <color rgb="FFC00000"/>
       </font>
@@ -834,14 +853,12 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
         <color theme="7" tint="-0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
         <strike val="0"/>
         <color rgb="FFC00000"/>
       </font>
@@ -849,7 +866,6 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
         <color theme="7" tint="-0.499984740745262"/>
       </font>
     </dxf>
@@ -1131,124 +1147,124 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22" ht="24" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>105</v>
+    <row r="1" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>107</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>108</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>112</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>114</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>115</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>116</v>
+        <v>12</v>
       </c>
       <c r="N1" s="2"/>
-      <c r="O1" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="20"/>
+      <c r="O1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="22"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
+      <c r="A2" s="19"/>
       <c r="B2" s="1" t="s">
-        <v>119</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>119</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>120</v>
+        <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>121</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>120</v>
+        <v>16</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>122</v>
+        <v>18</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>123</v>
+        <v>19</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>124</v>
+        <v>20</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>121</v>
+        <v>17</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>120</v>
+        <v>16</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="3" t="s">
-        <v>125</v>
+        <v>21</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>126</v>
+        <v>22</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>127</v>
+        <v>23</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>128</v>
+        <v>24</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>130</v>
+        <v>26</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>131</v>
+        <v>27</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>132</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -2608,65 +2624,65 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7EFB00C-8B25-4187-80B0-5E8B5E28C39B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:O61"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="A1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" s="17" t="s">
         <v>42</v>
-      </c>
-      <c r="N1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E2">
         <v>180</v>
@@ -2704,7 +2720,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E3">
         <v>180</v>
@@ -2742,7 +2758,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E4">
         <v>180</v>
@@ -2780,7 +2796,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E5">
         <v>180</v>
@@ -2818,7 +2834,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E6">
         <v>180</v>
@@ -2856,7 +2872,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E7">
         <v>180</v>
@@ -2894,7 +2910,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E8">
         <v>180</v>
@@ -2932,7 +2948,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E9">
         <v>180</v>
@@ -2970,7 +2986,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E10">
         <v>180</v>
@@ -3008,7 +3024,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E11">
         <v>180</v>
@@ -3046,7 +3062,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E12">
         <v>180</v>
@@ -3084,7 +3100,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E13">
         <v>180</v>
@@ -3122,7 +3138,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E14">
         <v>180</v>
@@ -3160,7 +3176,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E15">
         <v>180</v>
@@ -3198,7 +3214,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E16">
         <v>180</v>
@@ -3236,7 +3252,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E17">
         <v>180</v>
@@ -3274,7 +3290,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E18">
         <v>180</v>
@@ -3312,7 +3328,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E19">
         <v>180</v>
@@ -3350,7 +3366,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E20">
         <v>180</v>
@@ -3388,7 +3404,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E21">
         <v>180</v>
@@ -3426,7 +3442,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E22">
         <v>180</v>
@@ -3464,7 +3480,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E23">
         <v>180</v>
@@ -3502,7 +3518,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E24">
         <v>180</v>
@@ -3540,7 +3556,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E25">
         <v>180</v>
@@ -3578,7 +3594,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E26">
         <v>180</v>
@@ -3616,7 +3632,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E27">
         <v>180</v>
@@ -3654,7 +3670,7 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E28">
         <v>180</v>
@@ -3692,7 +3708,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E29">
         <v>180</v>
@@ -3730,7 +3746,7 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E30">
         <v>180</v>
@@ -3768,7 +3784,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E31">
         <v>180</v>
@@ -3806,7 +3822,7 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E32">
         <v>180</v>
@@ -3844,7 +3860,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E33">
         <v>180</v>
@@ -3882,7 +3898,7 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E34">
         <v>180</v>
@@ -3920,7 +3936,7 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E35">
         <v>180</v>
@@ -3958,7 +3974,7 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E36">
         <v>180</v>
@@ -3996,7 +4012,7 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E37">
         <v>180</v>
@@ -4034,7 +4050,7 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E38">
         <v>180</v>
@@ -4072,7 +4088,7 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E39">
         <v>180</v>
@@ -4110,7 +4126,7 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E40">
         <v>180</v>
@@ -4148,7 +4164,7 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E41">
         <v>180</v>
@@ -4186,7 +4202,7 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E42">
         <v>180</v>
@@ -4224,7 +4240,7 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E43">
         <v>180</v>
@@ -4262,7 +4278,7 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E44">
         <v>180</v>
@@ -4300,7 +4316,7 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E45">
         <v>180</v>
@@ -4338,7 +4354,7 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E46">
         <v>180</v>
@@ -4376,7 +4392,7 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E47">
         <v>180</v>
@@ -4414,7 +4430,7 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E48">
         <v>180</v>
@@ -4452,7 +4468,7 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E49">
         <v>180</v>
@@ -4490,7 +4506,7 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E50">
         <v>180</v>
@@ -4528,7 +4544,7 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E51">
         <v>180</v>
@@ -4566,7 +4582,7 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E52">
         <v>180</v>
@@ -4604,7 +4620,7 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E53">
         <v>180</v>
@@ -4642,7 +4658,7 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E54">
         <v>180</v>
@@ -4680,7 +4696,7 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E55">
         <v>180</v>
@@ -4718,7 +4734,7 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E56">
         <v>180</v>
@@ -4756,7 +4772,7 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E57">
         <v>180</v>
@@ -4794,7 +4810,7 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E58">
         <v>180</v>
@@ -4832,7 +4848,7 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E59">
         <v>180</v>
@@ -4870,7 +4886,7 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E60">
         <v>180</v>
@@ -4908,7 +4924,7 @@
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E61">
         <v>180</v>
@@ -4946,7 +4962,7 @@
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="E62">
         <v>180</v>
@@ -4984,7 +5000,7 @@
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
       <c r="E63">
         <v>180</v>
@@ -5022,7 +5038,7 @@
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="E64">
         <v>180</v>
@@ -5060,7 +5076,7 @@
     </row>
     <row r="65" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -5102,80 +5118,80 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4814A4E-B455-4FF3-8387-1272BD642410}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
+      <c r="A1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>123</v>
       </c>
       <c r="E2">
         <v>-3268.8759770000001</v>
@@ -5228,7 +5244,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>124</v>
       </c>
       <c r="E3">
         <v>-3228.648682</v>
@@ -5281,7 +5297,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="E4">
         <v>-3233.046875</v>
@@ -5334,7 +5350,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>126</v>
       </c>
       <c r="E5">
         <v>-3423.578857</v>
@@ -5387,7 +5403,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>127</v>
       </c>
       <c r="E6">
         <v>-3084.220703</v>
@@ -5440,7 +5456,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="E7">
         <v>617.49804700000004</v>
@@ -5493,7 +5509,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>129</v>
       </c>
       <c r="E8">
         <v>-170.87887599999999</v>
@@ -5546,7 +5562,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>130</v>
       </c>
       <c r="E9">
         <v>-171.50933800000001</v>
@@ -5599,7 +5615,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>131</v>
       </c>
       <c r="E10">
         <v>-171.58973700000001</v>
@@ -5652,7 +5668,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>132</v>
       </c>
       <c r="E11">
         <v>-170.915359</v>
@@ -5705,145 +5721,113 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="E12">
-        <f>MIN(E2:E11)</f>
         <v>-3423.578857</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12:T12" si="0">MIN(F2:F11)</f>
         <v>204.89872700000001</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
         <v>-2532.2983399999998</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
         <v>-213.00924699999999</v>
       </c>
       <c r="I12">
-        <f t="shared" si="0"/>
         <v>-3789.9104000000002</v>
       </c>
       <c r="J12">
-        <f t="shared" si="0"/>
         <v>-196.02848800000001</v>
       </c>
       <c r="K12">
-        <f t="shared" si="0"/>
         <v>-3613.194336</v>
       </c>
       <c r="L12">
-        <f t="shared" si="0"/>
         <v>-277.23291</v>
       </c>
       <c r="M12">
-        <f t="shared" si="0"/>
         <v>-5532.1806640000004</v>
       </c>
       <c r="N12">
-        <f t="shared" si="0"/>
         <v>-214.09491</v>
       </c>
       <c r="O12">
-        <f t="shared" si="0"/>
         <v>-4877.4711909999996</v>
       </c>
       <c r="P12">
-        <f t="shared" si="0"/>
         <v>-422.35528599999998</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="0"/>
         <v>-2467.6430660000001</v>
       </c>
       <c r="R12">
-        <f t="shared" si="0"/>
         <v>249.58215300000001</v>
       </c>
       <c r="S12">
-        <f t="shared" si="0"/>
         <v>-2559.6103520000001</v>
       </c>
       <c r="T12">
-        <f t="shared" si="0"/>
         <v>-82.410385000000005</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
       <c r="E13">
-        <f>MAX(E2:E11)</f>
         <v>617.49804700000004</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13:T13" si="1">MAX(F2:F11)</f>
         <v>5318.1352539999998</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
         <v>640.13641399999995</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
         <v>5747.1621089999999</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
         <v>551.88177499999995</v>
       </c>
       <c r="J13">
-        <f t="shared" si="1"/>
         <v>4191.7119140000004</v>
       </c>
       <c r="K13">
-        <f t="shared" si="1"/>
         <v>571.95495600000004</v>
       </c>
       <c r="L13">
-        <f t="shared" si="1"/>
         <v>4561.0864259999998</v>
       </c>
       <c r="M13">
-        <f t="shared" si="1"/>
         <v>584.494507</v>
       </c>
       <c r="N13">
-        <f t="shared" si="1"/>
         <v>5186.6479490000002</v>
       </c>
       <c r="O13">
-        <f t="shared" si="1"/>
         <v>667.87329099999999</v>
       </c>
       <c r="P13">
-        <f t="shared" si="1"/>
         <v>5966.3945309999999</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="1"/>
         <v>46.387596000000002</v>
       </c>
       <c r="R13">
-        <f t="shared" si="1"/>
         <v>2133.5351559999999</v>
       </c>
       <c r="S13">
-        <f t="shared" si="1"/>
         <v>362.10607900000002</v>
       </c>
       <c r="T13">
-        <f t="shared" si="1"/>
         <v>2663.0190429999998</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="E14">
         <v>-1710.7862399999999</v>
@@ -5896,7 +5880,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="E15">
         <v>1624.817364</v>

</xml_diff>